<commit_message>
Make it like a function
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="76">
   <si>
     <t>НАИМЕНОВАНИЕ ОРГАНИЗАЦИИ</t>
   </si>
@@ -29,319 +29,220 @@
     <t>ПРЕДЛОЖЕННАЯ ЦЕНА</t>
   </si>
   <si>
-    <t>Каракол-Аксуйское территориальное управление по землеустройству и регистрации прав на недвижимое имущество при ДКиРПНИ при ГРС</t>
-  </si>
-  <si>
-    <t>Учреждение Школа-гимназия №6 имени А. С. Макаренко</t>
-  </si>
-  <si>
-    <t>Филиал открытого акционерного общества Кыргызалтын санаторий Кыргызское Взморье</t>
-  </si>
-  <si>
-    <t>Муниципальное предприятие на праве хозяйственного ведения «Ноокат Водоканал»</t>
-  </si>
-  <si>
-    <t>Муниципальное предприятие "Дирекция рынков г. Ош"</t>
-  </si>
-  <si>
-    <t>Джетиогузский районный отдел образования Ысыккульской области</t>
-  </si>
-  <si>
-    <t>Автобаза Департамента здравоохранения мерии г. Бишкек</t>
-  </si>
-  <si>
-    <t>Аксы Кыргызпочта</t>
-  </si>
-  <si>
-    <t>Учреждение "Фрунзенская средняя школа-лицей № 1"</t>
-  </si>
-  <si>
-    <t>Учреждение "Фрунзенская средняя школа №2"</t>
-  </si>
-  <si>
-    <t>Ошское городское муниципальное автотранспортное предприятие</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ошское гор.управление по землеустройству и рег прав на недвижимое имущество Департамента кадастра и </t>
-  </si>
-  <si>
-    <t>Общество с ограниченной ответственностью КАСТА-СОБСТВЕННОСТИ</t>
-  </si>
-  <si>
-    <t>Общество с ограниченной ответственностью "Экспресс оценка"</t>
+    <t>Профессиональный лицей № 105</t>
+  </si>
+  <si>
+    <t>Филиал Автотранспортное предприятие  ОАО Кыргызалтын</t>
+  </si>
+  <si>
+    <t>Муниципальное предприятие "Бишкекглавархитектура"</t>
+  </si>
+  <si>
+    <t>Ошский филиал Государственного предприятие "Управление военной торговли Министерства обороны Кыргызской Республики"</t>
+  </si>
+  <si>
+    <t>Филиал "Ысык-Кол автовокзалы" при государственном предприятии «Кыргыз автобекети» Министерства транспорта и дорог Кыргызской Республики</t>
+  </si>
+  <si>
+    <t>Касымалиева Фатима Таштанкуловна</t>
+  </si>
+  <si>
+    <t>Бектуров Айдар Акимканович</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Байнур Групп"</t>
+  </si>
+  <si>
+    <t>Таласбеков Искендер Алмазович</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Арсен Трейд ЛТД"</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью  Максимус</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Береке Канц"</t>
+  </si>
+  <si>
+    <t>Каримкулова Юлия Витальевна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Токо кызы Каныкей </t>
+  </si>
+  <si>
+    <t>Отонбаева Мээрим Камчыбековна</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Мунар Фёрст"</t>
+  </si>
+  <si>
+    <t>Есенгельдиева Айпери Есенгельдиевна</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Мега Азия ЛЛТД"</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Нур Салам"</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Крот компани"</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Универсал плюс"</t>
+  </si>
+  <si>
+    <t>Капарова Акмарал Арапбаевна</t>
+  </si>
+  <si>
+    <t>Абдимиталип кызы Айсалкын</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Прогресс Тур Плюс"</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Нур универсал групп"</t>
   </si>
   <si>
     <t>Общество с ограниченной ответственностью "Алга Холдинг"</t>
   </si>
   <si>
-    <t>Алиева Гулбара Маматибраимовна</t>
-  </si>
-  <si>
-    <t>Айдаров Абдимиталип Омарович</t>
-  </si>
-  <si>
-    <t>Сатвалдиева Айсулуу Шарабидиновна</t>
-  </si>
-  <si>
-    <t>Открытое Акционерное Общество "Ош Сут"</t>
-  </si>
-  <si>
-    <t>Мамытов Каныбек Акматович</t>
-  </si>
-  <si>
-    <t>Каныбек уулу Байаман</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Закрытое   акционерное общество "Ак-Жалга"</t>
-  </si>
-  <si>
-    <t>Шимаров Шарба Рахимович</t>
-  </si>
-  <si>
-    <t>Общество с ограниченной ответсвенностью  " АЗИЯСНАБ"</t>
-  </si>
-  <si>
-    <t>Общество с ограниченной ответственностью "Нефтяная компания Сервис"</t>
-  </si>
-  <si>
-    <t>Мамаева Алмахан Салиевна</t>
-  </si>
-  <si>
-    <t>Ирисова Асель Рахматыллаевна</t>
-  </si>
-  <si>
-    <t>Общество с ограниченной ответственностью"Алакан-Строй"</t>
-  </si>
-  <si>
-    <t>Капарова Акмарал Арапбаевна</t>
-  </si>
-  <si>
-    <t>Общество с ограниченной ответственностью "КанцМир"</t>
-  </si>
-  <si>
-    <t>Абдимиталип кызы Айсалкын</t>
-  </si>
-  <si>
-    <t>Салижанов Мавлон Мамирович</t>
-  </si>
-  <si>
-    <t>Гайыпкулова Жыпаргул Талайбековна</t>
-  </si>
-  <si>
-    <t>Общество с ограниченной ответственностью "Ашан ЛТД"</t>
-  </si>
-  <si>
-    <t>Боронбаев Кубатбек Мамытович</t>
-  </si>
-  <si>
-    <t>Кочобаева Кулжамал Аралакуновна</t>
-  </si>
-  <si>
-    <t>Общество с ограниченной ответственностью "Империал Холдинг"</t>
-  </si>
-  <si>
-    <t>Иманкулов Нурлан Мухамедович</t>
-  </si>
-  <si>
-    <t>Общество с ограниченной ответственностью "Фарватер"</t>
-  </si>
-  <si>
-    <t>Джапарова Жанар Алиакбаровна</t>
-  </si>
-  <si>
-    <t>Сармырзаева Жыпар Дуйшеналиевна</t>
-  </si>
-  <si>
-    <t>Общество с ограниченной ответственностью "НТД Групп"</t>
-  </si>
-  <si>
-    <t>Василенко Тамара Сергеевна</t>
-  </si>
-  <si>
-    <t>Ашимова Салтанат Камчибековна</t>
-  </si>
-  <si>
-    <t>Осмонова Кулмайра Джузубековна</t>
-  </si>
-  <si>
-    <t>Общество с ограниченной ответственностью "РОССИЯ Нефть"</t>
-  </si>
-  <si>
-    <t>Общество с ограниченной ответственностью "ПАРТНЕР НЕФТЬ"</t>
-  </si>
-  <si>
-    <t>Аскарова Инаят</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L001-01 : переоценка основных фондов движимого и не движимого имущества                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L001-01 : Булочка сдобные,пряники глазированные, печенье песочное, кекс, коржики молочные.                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L003-01 : Молоко коровье пастеризованное 2,5 % жирности.                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L004-01 : Сухофрукты из абрикоса (орук)                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L002-01 : Лоту №2 Молочные продукты                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L006-01 : Лот №7 Овощи                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L003-01 : Лот №3-Бакалейные и сыпучие товары                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L001-01 : Приобретение ГСМ                                    </t>
+    <t>Общество с ограниченной ответственностью "Арча Групп"</t>
+  </si>
+  <si>
+    <t>Асаналиев Стал Темирбекович</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "КейДжи Трэйдинг Компани"</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Флай Тайм"</t>
+  </si>
+  <si>
+    <t>Сапаров Уланбек Турдакунович</t>
+  </si>
+  <si>
+    <t>Амангелдиева Чолпон Талантбековна</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Бренден"</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "АйкурКомпани"</t>
+  </si>
+  <si>
+    <t>Исраилова Махабат Исмаиловна</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Ызат и Ко"</t>
+  </si>
+  <si>
+    <t>Общество с ограниченной ответственностью "Элементал"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L001-01 : Продовольственные товары.                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L001-01 : Канцтовары и компьютерные принадлежности                                    </t>
   </si>
   <si>
     <t xml:space="preserve">L001-01 : Канцелярские товары                                    </t>
   </si>
   <si>
-    <t xml:space="preserve">L001-01 : 2218-школы                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L001-01 : Гипс                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L001-01 : АИ - 92                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L001-01 : Продукты питания                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L001-01 : Продукты питания                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L001-01 : топливо                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L001-01 : Приобретение канцелярских товаров за 1-квартал 2019 года                                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 000                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 500                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 900                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">384 480                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">376 470                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">535 068                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">86 508                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">67 120,2                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">71 686,2                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">338 500                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">160 000                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">659 985                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">66 375                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">39 670                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">57 220                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">50 210                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">49 680                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">37 900                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">48 800                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">51 790                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">42 520                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">47 900                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">40 520                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">999 025                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">999 904                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 990                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 000                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">35 000                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">49 450                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">268 195                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">290 510                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">283 260                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">257 115                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">163 000                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">153 000                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">148 300                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 712 640                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 589 450                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">68 500                                    </t>
+    <t xml:space="preserve">L001-01 : Покупка подшипников                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L002-01 : Электротовары                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">262 300                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">xxxxxx                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">600 000                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">524 350                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">603 730                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">553 905                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">678 600                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">547 450                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">427 215                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">690 000                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">486 850                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">662 425                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">639 000                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">632 775                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 380                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 450                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 280                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">71 000                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 170                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 300                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 200                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 400                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 368                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 400                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 840                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 990                                    </t>
   </si>
   <si>
     <t xml:space="preserve">65 600                                    </t>
   </si>
   <si>
-    <t xml:space="preserve">67 700                                    </t>
+    <t xml:space="preserve">21 460                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 700                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 180                                    </t>
   </si>
 </sst>
 </file>
@@ -699,7 +600,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -727,13 +628,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -744,13 +645,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -758,16 +659,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -775,16 +676,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -792,16 +693,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -809,16 +710,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -826,16 +727,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -843,16 +744,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -860,16 +761,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -877,16 +778,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
         <v>53</v>
-      </c>
-      <c r="E11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -894,16 +795,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
         <v>54</v>
-      </c>
-      <c r="E12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -911,16 +812,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
         <v>55</v>
-      </c>
-      <c r="E13" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -928,16 +829,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -948,13 +849,13 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -965,13 +866,13 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -982,13 +883,13 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -999,13 +900,13 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1016,13 +917,13 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1030,16 +931,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1050,13 +951,13 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1067,13 +968,13 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1084,13 +985,13 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1101,13 +1002,13 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1118,13 +1019,13 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1135,13 +1036,13 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1152,13 +1053,13 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1169,13 +1070,13 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1186,13 +1087,13 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1200,16 +1101,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1217,16 +1118,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E31" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1234,16 +1135,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E32" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1251,16 +1152,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E33" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1268,16 +1169,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E34" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1285,16 +1186,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1302,16 +1203,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E36" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1319,16 +1220,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E37" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1336,16 +1237,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D38" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="E38" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1353,16 +1254,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D39" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="E39" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1370,16 +1271,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D40" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="E40" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1387,16 +1288,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="E41" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1404,16 +1305,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="E42" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1421,16 +1322,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D43" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="E43" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1438,16 +1339,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="E44" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1455,16 +1356,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D45" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="E45" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1472,16 +1373,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D46" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="E46" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1489,16 +1390,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="E47" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1506,16 +1407,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="E48" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1523,16 +1424,101 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="D49" t="s">
-        <v>67</v>
-      </c>
-      <c r="E49" t="s">
-        <v>108</v>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" t="s">
+        <v>44</v>
+      </c>
+      <c r="E54" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1542,7 +1528,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1570,189 +1556,205 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D9" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D11" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D18" s="1" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1760,225 +1762,183 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1"/>
-      <c r="B26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1"/>
-      <c r="B28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1"/>
-      <c r="B29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1"/>
-      <c r="B31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1"/>
-      <c r="B34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1"/>
-      <c r="B35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1986,184 +1946,205 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1"/>
-      <c r="B40" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1"/>
-      <c r="B41" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1"/>
-      <c r="B43" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1"/>
-      <c r="B44" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1"/>
-      <c r="B46" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1"/>
-      <c r="B49" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>108</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A5:A14"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A20:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C36:C37"/>
+  <mergeCells count="30">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A5:A18"/>
+    <mergeCell ref="A21:A54"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="C53:C54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>